<commit_message>
Ajuste na organização dos servidores da estrututra
</commit_message>
<xml_diff>
--- a/funcionarios.xlsx
+++ b/funcionarios.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdpuser\Desktop\PROJETOS\organograma-atribuicoes-cogespa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.vargas\Desktop\PROJETOS\organograma-atribuicoes-cogespa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4D38F2-031E-4726-AC55-6F533E223030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE2DC93-D7FC-4659-A963-D39A648492EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$I$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$I$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Planilha1!$A$1:$D$66</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Plan1!$B$1:$I$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Plan1!$B$1:$I$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="142">
   <si>
     <t xml:space="preserve">NOME </t>
   </si>
@@ -356,9 +356,6 @@
     <t>ADRIANO DOS SANTOS CHAVES</t>
   </si>
   <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
     <t>01 a 15</t>
   </si>
   <si>
@@ -383,12 +380,6 @@
     <t>01 a 12    28 a 31</t>
   </si>
   <si>
-    <t>16 a 30</t>
-  </si>
-  <si>
-    <t>01 a 15    31</t>
-  </si>
-  <si>
     <t>21 a 04/11</t>
   </si>
   <si>
@@ -414,21 +405,6 @@
   </si>
   <si>
     <t xml:space="preserve">DGPDOC/AROUCHE                      </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">COGESPA/COPROG                            </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">DPGDOC                       </t>
@@ -703,6 +679,24 @@
   </si>
   <si>
     <t xml:space="preserve">DPGDOC           </t>
+  </si>
+  <si>
+    <t>DPGDOC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">COGESPA/COEX             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1061,12 +1055,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" sqref="A1:I66"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1078,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1113,240 +1107,240 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" t="s">
         <v>105</v>
-      </c>
-      <c r="I4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I10" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I15" t="s">
         <v>110</v>
@@ -1354,673 +1348,667 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" t="s">
-        <v>118</v>
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>96</v>
       </c>
       <c r="I21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
       </c>
       <c r="I22" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="I23" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I24" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I26" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
       </c>
       <c r="I27" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>102</v>
       </c>
       <c r="I28" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I29" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
         <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="I30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="I31" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>102</v>
       </c>
       <c r="I33" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="I34" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="I35" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="I36" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I37" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="I38" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
         <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I39" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I40" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I41" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="E42" t="s">
+        <v>90</v>
       </c>
       <c r="I42" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I43" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="D44" t="s">
-        <v>92</v>
-      </c>
-      <c r="E44" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="I44" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="D45" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="I45" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I46" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="D47" t="s">
+        <v>102</v>
       </c>
       <c r="I47" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
         <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I48" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" t="s">
         <v>56</v>
       </c>
-      <c r="B49" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" t="s">
-        <v>71</v>
-      </c>
       <c r="I49" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D50" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I50" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>31</v>
+      </c>
+      <c r="D51" t="s">
+        <v>102</v>
       </c>
       <c r="I51" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>96</v>
-      </c>
-      <c r="E52" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="I52" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="D53" t="s">
         <v>102</v>
       </c>
-      <c r="E53" t="s">
-        <v>101</v>
-      </c>
       <c r="I53" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D54" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I54" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I55" t="s">
         <v>125</v>
@@ -2028,199 +2016,123 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>105</v>
+        <v>93</v>
+      </c>
+      <c r="E56" t="s">
+        <v>92</v>
       </c>
       <c r="I56" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>28</v>
+      </c>
+      <c r="D57" t="s">
+        <v>102</v>
       </c>
       <c r="I57" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D58" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="E58" t="s">
+        <v>98</v>
       </c>
       <c r="I58" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D59" t="s">
-        <v>90</v>
-      </c>
-      <c r="E59" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="I59" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E60" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I60" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C61" t="s">
         <v>71</v>
       </c>
       <c r="D61" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I61" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>70</v>
-      </c>
-      <c r="B62" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I62" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>71</v>
-      </c>
-      <c r="B63" t="s">
-        <v>52</v>
-      </c>
-      <c r="C63" t="s">
-        <v>55</v>
-      </c>
-      <c r="D63" t="s">
-        <v>105</v>
-      </c>
-      <c r="I63" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>72</v>
-      </c>
-      <c r="B64" t="s">
-        <v>53</v>
-      </c>
-      <c r="C64" t="s">
-        <v>71</v>
-      </c>
-      <c r="D64" t="s">
-        <v>98</v>
-      </c>
-      <c r="E64" t="s">
-        <v>97</v>
-      </c>
-      <c r="I64" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>73</v>
-      </c>
-      <c r="B65" t="s">
-        <v>54</v>
-      </c>
-      <c r="C65" t="s">
-        <v>71</v>
-      </c>
-      <c r="D65" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>74</v>
-      </c>
-      <c r="B66" t="s">
-        <v>87</v>
-      </c>
-      <c r="C66" t="s">
-        <v>55</v>
-      </c>
-      <c r="D66" t="s">
-        <v>105</v>
-      </c>
-      <c r="I66" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" caseSensitive="1" ref="A2:I67">
-    <sortCondition ref="A1:A67"/>
+  <autoFilter ref="A1:I61" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I61">
+      <sortCondition ref="B1:B61"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" caseSensitive="1" ref="A2:I61">
+    <sortCondition ref="A1:A61"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
@@ -2231,7 +2143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92D1F0D-A188-4CFA-8D8A-838F3B921914}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2245,7 +2157,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2268,7 +2180,7 @@
         <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,7 +2194,7 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,7 +2208,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,7 +2222,7 @@
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,7 +2236,7 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,7 +2250,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,7 +2264,7 @@
         <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,7 +2278,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,7 +2292,7 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,7 +2306,7 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2408,7 +2320,7 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,7 +2334,7 @@
         <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2436,7 +2348,7 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2450,7 +2362,7 @@
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,7 +2376,7 @@
         <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2478,7 +2390,7 @@
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2492,7 +2404,7 @@
         <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2506,7 +2418,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2520,7 +2432,7 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2534,7 +2446,7 @@
         <v>62</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2548,7 +2460,7 @@
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2562,7 +2474,7 @@
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2576,7 +2488,7 @@
         <v>28</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2590,7 +2502,7 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2604,7 +2516,7 @@
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2618,7 +2530,7 @@
         <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2632,7 +2544,7 @@
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2646,7 +2558,7 @@
         <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2660,7 +2572,7 @@
         <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,7 +2586,7 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2688,7 +2600,7 @@
         <v>28</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2716,7 +2628,7 @@
         <v>56</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2730,7 +2642,7 @@
         <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2744,7 +2656,7 @@
         <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2758,7 +2670,7 @@
         <v>73</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,7 +2698,7 @@
         <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,7 +2712,7 @@
         <v>28</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2814,7 +2726,7 @@
         <v>72</v>
       </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2828,7 +2740,7 @@
         <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2842,7 +2754,7 @@
         <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2856,7 +2768,7 @@
         <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2870,7 +2782,7 @@
         <v>72</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2884,7 +2796,7 @@
         <v>29</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2912,7 +2824,7 @@
         <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2926,7 +2838,7 @@
         <v>71</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2940,7 +2852,7 @@
         <v>82</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2954,7 +2866,7 @@
         <v>72</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2968,7 +2880,7 @@
         <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2996,7 +2908,7 @@
         <v>55</v>
       </c>
       <c r="D54" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3010,7 +2922,7 @@
         <v>71</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3024,7 +2936,7 @@
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3052,7 +2964,7 @@
         <v>72</v>
       </c>
       <c r="D58" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3066,7 +2978,7 @@
         <v>71</v>
       </c>
       <c r="D59" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3080,7 +2992,7 @@
         <v>72</v>
       </c>
       <c r="D60" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3094,7 +3006,7 @@
         <v>71</v>
       </c>
       <c r="D61" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3122,7 +3034,7 @@
         <v>55</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3150,7 +3062,7 @@
         <v>71</v>
       </c>
       <c r="D65" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3164,7 +3076,7 @@
         <v>55</v>
       </c>
       <c r="D66" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3182,15 +3094,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E4B2DE180F272240A2146569C9A90399" ma:contentTypeVersion="15" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="0578d45eed8a5920582b5b08aae5857c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d85f143d-11f6-4ef3-a558-24ab759f3d10" xmlns:ns4="a080b25b-87c9-49fc-939f-e37ee00c292b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a2cb74cf232f876297862cbc20f9b4c" ns3:_="" ns4:_="">
     <xsd:import namespace="d85f143d-11f6-4ef3-a558-24ab759f3d10"/>
@@ -3423,6 +3326,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E1D71B6-36E3-4129-9177-6C975CB6BFAD}">
   <ds:schemaRefs>
@@ -3441,14 +3353,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD53C6DC-F67B-4B6F-8F63-122F57958613}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B95EB1E-55A7-457E-9DB3-F97D4C410F70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3465,4 +3369,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD53C6DC-F67B-4B6F-8F63-122F57958613}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>